<commit_message>
feat(chooseSemester): Choose the semester you want to get curriculum from
</commit_message>
<xml_diff>
--- a/Curriculum.xlsx
+++ b/Curriculum.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,118 +466,518 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>形势与政策-6</t>
+          <t>体育-3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>马力</t>
+          <t>ty9</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>江安一教B座B207</t>
+          <t>江安体育场体育场2号</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>107120000</t>
+          <t>888006010</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>09</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>11,13,15,17周上</t>
+          <t>2-17周</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>大数据技术原理与应用</t>
+          <t>形势与政策-3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>耿天玉</t>
+          <t>刘辉</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>江安一教A座A507</t>
+          <t>江安综合楼C座C306</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>304213020</t>
+          <t>107117000</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1-16周</t>
+          <t>3-9周单</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>大数据技术原理与应用实践</t>
+          <t>马克思主义基本原理概论</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>肖蓉</t>
+          <t>陈伟</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>江安实验室二基楼B300</t>
+          <t>江安综合楼C座C403</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>304220030</t>
+          <t>107021030</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2-18周</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>JAVA程序设计</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>李琳</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>江安一教B座B203</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>304007030</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2-17周</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>大学英语（创意阅读）-3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>徐光源</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>江安一教A座A203</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>105395020</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2-18周</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>物联网工程导论</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>桑永胜</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>江安一教A座A506</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>304085010</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>01</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1-16周</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2-9周</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>物联网传感器原理及应用</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>时宏伟</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>江安一教C座C504</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>304211030</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2-9周</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>计算机组成原理实验</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>蒋欣荣</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>江安实验室二基楼B310B</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>304037010</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>11-15周</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>离散数学</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>陈瑜</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>江安综合楼C座C303</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>304156050</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2-18周</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>离散数学</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>陈瑜</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>江安一教B座B201</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>304156050</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2-18周</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>计算机组成原理</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>蒋欣荣</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>江安综合楼C座C408</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>304036030</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2-17周</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>数据结构与算法分析课程设计</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>周欣</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>江安实验室二基楼B304</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>304046010</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>6-15周</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>4</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>数据结构与算法分析</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>周欣</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>江安一教C座C406</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>304045030</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2-17周</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>3</t>
         </is>

</xml_diff>